<commit_message>
Implements all maps and mouse switch for maps
</commit_message>
<xml_diff>
--- a/Dantong Xue_Sprint0/Game1/Game1/Maps/test_colored.xlsx
+++ b/Dantong Xue_Sprint0/Game1/Game1/Maps/test_colored.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repo\CSE-3902\Dantong Xue_Sprint0\Game1\Game1\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A94FBE-36AD-4A65-B47F-4CF1A66653EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2446BFE1-C3ED-4B1E-8D66-17F48CF0DDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="7">
   <si>
     <t>lockedDoorFront</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -47,10 +47,6 @@
   </si>
   <si>
     <t>wall_2</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>water</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -781,7 +777,58 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,58 +858,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1223,7 +1219,7 @@
   <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9:Z10"/>
+      <selection activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1232,44 +1228,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="12" t="s">
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="14"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="4"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1290,38 +1286,38 @@
       <c r="AX1" s="1"/>
     </row>
     <row r="2" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="17"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="7"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -1342,38 +1338,38 @@
       <c r="AX2" s="1"/>
     </row>
     <row r="3" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="16"/>
-      <c r="AD3" s="16"/>
-      <c r="AE3" s="16"/>
-      <c r="AF3" s="17"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="7"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -1394,38 +1390,38 @@
       <c r="AX3" s="1"/>
     </row>
     <row r="4" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="20"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="10"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1446,66 +1442,66 @@
       <c r="AX4" s="1"/>
     </row>
     <row r="5" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="3" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="5"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="22"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1526,38 +1522,38 @@
       <c r="AX5" s="1"/>
     </row>
     <row r="6" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="8"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="25"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1578,62 +1574,62 @@
       <c r="AX6" s="1"/>
     </row>
     <row r="7" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="8"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="24"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="25"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
@@ -1654,38 +1650,38 @@
       <c r="AX7" s="1"/>
     </row>
     <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="8"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="25"/>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -1706,62 +1702,62 @@
       <c r="AX8" s="1"/>
     </row>
     <row r="9" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="11"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="28"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
@@ -1782,42 +1778,42 @@
       <c r="AX9" s="1"/>
     </row>
     <row r="10" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="21" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="22"/>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="23"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="13"/>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
@@ -1838,62 +1834,62 @@
       <c r="AX10" s="1"/>
     </row>
     <row r="11" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="25"/>
-      <c r="AE11" s="25"/>
-      <c r="AF11" s="26"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="16"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -1914,38 +1910,38 @@
       <c r="AX11" s="1"/>
     </row>
     <row r="12" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="25"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="26"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="16"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
@@ -1966,62 +1962,62 @@
       <c r="AX12" s="1"/>
     </row>
     <row r="13" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="29"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="19"/>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
@@ -2042,42 +2038,42 @@
       <c r="AX13" s="1"/>
     </row>
     <row r="14" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="3" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="5"/>
+      <c r="AD14" s="21"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="22"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
@@ -2098,62 +2094,62 @@
       <c r="AX14" s="1"/>
     </row>
     <row r="15" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="8"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="25"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
@@ -2174,38 +2170,38 @@
       <c r="AX15" s="1"/>
     </row>
     <row r="16" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="8"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="25"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -2226,62 +2222,62 @@
       <c r="AX16" s="1"/>
     </row>
     <row r="17" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="8"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="25"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2302,38 +2298,38 @@
       <c r="AX17" s="1"/>
     </row>
     <row r="18" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="11"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="28"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2354,44 +2350,44 @@
       <c r="AX18" s="1"/>
     </row>
     <row r="19" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="21" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="12" t="s">
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="14"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="4"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2412,38 +2408,38 @@
       <c r="AX19" s="1"/>
     </row>
     <row r="20" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="16"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
-      <c r="AC20" s="16"/>
-      <c r="AD20" s="16"/>
-      <c r="AE20" s="16"/>
-      <c r="AF20" s="17"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="7"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -2464,38 +2460,38 @@
       <c r="AX20" s="1"/>
     </row>
     <row r="21" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="16"/>
-      <c r="AD21" s="16"/>
-      <c r="AE21" s="16"/>
-      <c r="AF21" s="17"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="7"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2516,38 +2512,38 @@
       <c r="AX21" s="1"/>
     </row>
     <row r="22" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="19"/>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="20"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="10"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
@@ -2985,6 +2981,86 @@
     </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="AA5:AB6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="Q5:R6"/>
+    <mergeCell ref="S5:T6"/>
+    <mergeCell ref="U5:V6"/>
+    <mergeCell ref="W5:X6"/>
+    <mergeCell ref="Y5:Z6"/>
+    <mergeCell ref="AA7:AB8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="Q7:R8"/>
+    <mergeCell ref="S7:T8"/>
+    <mergeCell ref="U7:V8"/>
+    <mergeCell ref="W7:X8"/>
+    <mergeCell ref="Y7:Z8"/>
+    <mergeCell ref="AA9:AB10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="Q9:R10"/>
+    <mergeCell ref="S9:T10"/>
+    <mergeCell ref="U9:V10"/>
+    <mergeCell ref="W9:X10"/>
+    <mergeCell ref="Y9:Z10"/>
+    <mergeCell ref="AA11:AB12"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="S11:T12"/>
+    <mergeCell ref="U11:V12"/>
+    <mergeCell ref="W11:X12"/>
+    <mergeCell ref="Y11:Z12"/>
+    <mergeCell ref="AA13:AB14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="Q13:R14"/>
+    <mergeCell ref="S13:T14"/>
+    <mergeCell ref="U13:V14"/>
+    <mergeCell ref="W13:X14"/>
+    <mergeCell ref="Y13:Z14"/>
+    <mergeCell ref="U17:V18"/>
+    <mergeCell ref="W17:X18"/>
+    <mergeCell ref="Y17:Z18"/>
+    <mergeCell ref="AA15:AB16"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="M15:N16"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="S15:T16"/>
+    <mergeCell ref="U15:V16"/>
+    <mergeCell ref="W15:X16"/>
+    <mergeCell ref="Y15:Z16"/>
+    <mergeCell ref="K17:L18"/>
+    <mergeCell ref="M17:N18"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="Q17:R18"/>
+    <mergeCell ref="S17:T18"/>
     <mergeCell ref="A19:N22"/>
     <mergeCell ref="S19:AF22"/>
     <mergeCell ref="O19:R22"/>
@@ -3001,86 +3077,6 @@
     <mergeCell ref="E17:F18"/>
     <mergeCell ref="G17:H18"/>
     <mergeCell ref="I17:J18"/>
-    <mergeCell ref="K17:L18"/>
-    <mergeCell ref="M17:N18"/>
-    <mergeCell ref="O17:P18"/>
-    <mergeCell ref="Q17:R18"/>
-    <mergeCell ref="S17:T18"/>
-    <mergeCell ref="U17:V18"/>
-    <mergeCell ref="W17:X18"/>
-    <mergeCell ref="Y17:Z18"/>
-    <mergeCell ref="AA15:AB16"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="M15:N16"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="S15:T16"/>
-    <mergeCell ref="U15:V16"/>
-    <mergeCell ref="W15:X16"/>
-    <mergeCell ref="Y15:Z16"/>
-    <mergeCell ref="AA13:AB14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="O13:P14"/>
-    <mergeCell ref="Q13:R14"/>
-    <mergeCell ref="S13:T14"/>
-    <mergeCell ref="U13:V14"/>
-    <mergeCell ref="W13:X14"/>
-    <mergeCell ref="Y13:Z14"/>
-    <mergeCell ref="AA11:AB12"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="S11:T12"/>
-    <mergeCell ref="U11:V12"/>
-    <mergeCell ref="W11:X12"/>
-    <mergeCell ref="Y11:Z12"/>
-    <mergeCell ref="AA9:AB10"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="S9:T10"/>
-    <mergeCell ref="U9:V10"/>
-    <mergeCell ref="W9:X10"/>
-    <mergeCell ref="Y9:Z10"/>
-    <mergeCell ref="AA7:AB8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="Q7:R8"/>
-    <mergeCell ref="S7:T8"/>
-    <mergeCell ref="U7:V8"/>
-    <mergeCell ref="W7:X8"/>
-    <mergeCell ref="Y7:Z8"/>
-    <mergeCell ref="AA5:AB6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="O5:P6"/>
-    <mergeCell ref="Q5:R6"/>
-    <mergeCell ref="S5:T6"/>
-    <mergeCell ref="U5:V6"/>
-    <mergeCell ref="W5:X6"/>
-    <mergeCell ref="Y5:Z6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>